<commit_message>
HP added to weekly content
</commit_message>
<xml_diff>
--- a/weekly_content/weekly_content_plan_HP.xlsx
+++ b/weekly_content/weekly_content_plan_HP.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/hp12384_bristol_ac_uk/Documents/Teaching/UoB/EMAT10007_2023/weekly_content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{F2FCDE39-672E-0044-9EAE-42FF74C13228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D32EE262-A395-DA4A-8B4C-98F09B023A4A}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{F2FCDE39-672E-0044-9EAE-42FF74C13228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0EFBB84-5DF0-6647-A868-3E9CDC4101E6}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="500" windowWidth="28040" windowHeight="15920" xr2:uid="{228F261D-1DF1-9344-81D9-2AC7985BA606}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,13 +56,6 @@
     <t xml:space="preserve">If, elif, else , netsed conditionals </t>
   </si>
   <si>
-    <t xml:space="preserve">1. A set of if statements (point to where to find more help in the hint)
-2. A set of if/else statements
-3. if/elif/else
-4. multiple elif (what's the correct order?)
-5. Open ended question - text based adventure game - get a friend or TA to play it or send it to me! </t>
-  </si>
-  <si>
     <t xml:space="preserve">Loops </t>
   </si>
   <si>
@@ -135,6 +128,14 @@
 3. Evaluating a problem with comparison and identity operators (circles)
 4. Logical operators
 5. Open-ended question </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A set of if statements (point to where to find more help in the hint)
+2. A set of if/else statements
+3. if/elif/else (earth layers)
+nested conditionals 
+4. multiple elif (what's the correct order?)
+5. Open ended question - text based adventure game - get a friend or TA to play it or send it to me! </t>
   </si>
 </sst>
 </file>
@@ -507,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B32DEA-1650-CD42-A3E3-11EF7C9273BC}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,16 +536,16 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="170" x14ac:dyDescent="0.2">
@@ -555,24 +556,24 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="204" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>